<commit_message>
changes to BOM for manufacturing
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://quantumhti.sharepoint.com/sites/company/Shared Documents/Quantum Integration/Engineering/Quantum Hardware/DIY Kits/Q-PCB-001/9V Rev G/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{49EE4D52-1356-114E-BC89-81BF49034CCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8BFF7362-17C1-A443-91DC-DF216496E935}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{49EE4D52-1356-114E-BC89-81BF49034CCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{76081EE6-D6F2-4E47-835B-01021B3706EF}"/>
   <bookViews>
-    <workbookView xWindow="58700" yWindow="460" windowWidth="25600" windowHeight="28340" xr2:uid="{E11B78B7-CBD0-0547-AFF9-37277F972DF5}"/>
+    <workbookView xWindow="51220" yWindow="3900" windowWidth="25600" windowHeight="28300" xr2:uid="{E11B78B7-CBD0-0547-AFF9-37277F972DF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,9 +105,6 @@
     <t>Electrolytic Capacitor</t>
   </si>
   <si>
-    <t>100n</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
   </si>
   <si>
     <t>6mm</t>
+  </si>
+  <si>
+    <t>220n</t>
   </si>
 </sst>
 </file>
@@ -643,7 +643,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -758,22 +758,22 @@
         <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -784,22 +784,22 @@
         <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -807,19 +807,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -827,7 +827,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1">
         <v>240</v>
@@ -836,16 +836,16 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="I8" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -853,7 +853,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1">
         <v>330</v>
@@ -862,16 +862,16 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="I9" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -879,7 +879,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1">
         <v>390</v>
@@ -888,16 +888,16 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="I10" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -905,25 +905,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="F11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="I11" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -931,22 +931,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="I12" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -954,22 +954,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="I13" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -977,22 +977,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="I14" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1000,22 +1000,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" s="1">
         <v>3</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F15" s="1">
         <v>0.1</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1023,16 +1023,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16" s="1">
         <v>3</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1040,16 +1040,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="I17" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1057,16 +1057,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1" t="s">
+      <c r="I18" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1074,13 +1074,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1088,16 +1088,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
-      <c r="G20" s="1" t="s">
+      <c r="I20" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1344,18 +1344,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1378,26 +1378,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F46DBAAA-4D3A-4026-9049-CAAAC23F78E1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ED18E5C-7CF9-4494-98F8-0E2F5EED4C77}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="97031774-c0c7-48a9-a8e1-3722ddd0f879"/>
-    <ds:schemaRef ds:uri="a32bd177-85eb-4316-9671-26122bedec74"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ED18E5C-7CF9-4494-98F8-0E2F5EED4C77}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F46DBAAA-4D3A-4026-9049-CAAAC23F78E1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a32bd177-85eb-4316-9671-26122bedec74"/>
+    <ds:schemaRef ds:uri="97031774-c0c7-48a9-a8e1-3722ddd0f879"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>